<commit_message>
Update TOPNET-Sprint Backlog scoring.xlsx
Co-Authored-By: Nacib Mariem <67750731+Nacib1999@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Conception Du Projet/TOPNET-Sprint Backlog scoring.xlsx
+++ b/Conception Du Projet/TOPNET-Sprint Backlog scoring.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Topnet-B2C-Stage-\Conception Du Projet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF1E5AC0-B158-4E18-BA86-68B6934E5BD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74182992-6FC3-4BF7-B728-427563971BAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="128">
   <si>
     <t>Theme</t>
   </si>
@@ -76,9 +76,6 @@
     <t>Délai moyen de paiement</t>
   </si>
   <si>
-    <t>Comportement client</t>
-  </si>
-  <si>
     <t>incident de paiement</t>
   </si>
   <si>
@@ -166,19 +163,10 @@
     <t xml:space="preserve">                Client Prespective</t>
   </si>
   <si>
-    <t xml:space="preserve">                 Authentification</t>
-  </si>
-  <si>
-    <t>Authentification</t>
-  </si>
-  <si>
     <t>Statut</t>
   </si>
   <si>
     <t xml:space="preserve">A Faire </t>
-  </si>
-  <si>
-    <t xml:space="preserve">En tant qu'utilisateur du  Topnet, je souhaite pouvoir m'authentifier en fournissant mes identifiants (nom d'utilisateur et mot de passe) pour accéder aux fonctionnalités sécurisées et confidentielles. </t>
   </si>
   <si>
     <t xml:space="preserve">                    Niveau Utilisateur</t>
@@ -236,10 +224,6 @@
 •Je veux ensuite pouvoir consulter ma catégorie client et voir les critères spécifiques utilisés pour me classer dans cette catégorie.</t>
   </si>
   <si>
-    <t>•Je veux pouvoir saisir mon nom d'utilisateur et mon mot de passe sur une page d'authentification.
-•Je souhaite que mes identifiants soient vérifiés et que j'accède aux fonctionnalités sécurisées une fois authentifié.</t>
-  </si>
-  <si>
     <t>Label</t>
   </si>
   <si>
@@ -283,9 +267,6 @@
   </si>
   <si>
     <t>CP-I-1</t>
-  </si>
-  <si>
-    <t>AUTH-I-1</t>
   </si>
   <si>
     <t>•Je souhaite pouvoir déterminer les critères d'offre, tels que le type de service (XDSL, HD).
@@ -298,6 +279,175 @@
   <si>
     <t>•Je veux pouvoir déterminer les critères d'engagement contractuel (par exemple : période d'engagement, non engagé) .
 •Je souhaite ensuite valider si le client est actuellement dans sa période d'engagement ou non.</t>
+  </si>
+  <si>
+    <t>C+A11:H13omportement client</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Authentification </t>
+  </si>
+  <si>
+    <t>Authentification de l'Agent</t>
+  </si>
+  <si>
+    <t>Authentification du Client</t>
+  </si>
+  <si>
+    <t>Gestion des comptes d'utilisateur</t>
+  </si>
+  <si>
+    <t>AUTH-A-1</t>
+  </si>
+  <si>
+    <t>AUTH-A-2</t>
+  </si>
+  <si>
+    <t>AUTH-A-3</t>
+  </si>
+  <si>
+    <t>En tant qu'agent du Topnet, je souhaite pouvoir m'authentifier en fournissant mes identifiants (nom d'utilisateur et mot de passe) pour accéder aux fonctionnalités sécurisées et confidentielles réservées aux agents.</t>
+  </si>
+  <si>
+    <t>• Je veux pouvoir saisir mon nom d'utilisateur et mon mot de passe sur une page d'authentification.
+• Je souhaite que mes identifiants soient vérifiés et que j'accède aux fonctionnalités sécurisées une fois authentifié.</t>
+  </si>
+  <si>
+    <t>En tant que client du Topnet, je souhaite pouvoir m'authentifier en fournissant mes identifiants (nom d'utilisateur et mot de passe) pour accéder à mon compte et à mes informations personnelles de manière sécurisée.</t>
+  </si>
+  <si>
+    <t>• Je souhaite pouvoir me connecter à mon compte en fournissant mes identifiants (nom d'utilisateur et mot de passe) pour accéder à mon profil.
+• Je veux ensuite pouvoir consulter ma catégorie client et voir les critères spécifiques utilisés pour me classer dans cette catégorie.</t>
+  </si>
+  <si>
+    <t>En tant qu'administrateur du Topnet, je souhaite pouvoir gérer les comptes d'utilisateurs, y compris la création, la modification et la suppression des comptes, afin de maintenir un contrôle sur les accès au système.</t>
+  </si>
+  <si>
+    <t>• Je veux pouvoir créer de nouveaux comptes d'utilisateurs en fournissant les informations nécessaires (nom, rôle, mot de passe, etc.).
+• Je souhaite pouvoir modifier les informations des comptes existants, tels que les rôles ou les autorisations.
+• Je veux pouvoir supprimer des comptes d'utilisateurs non nécessaires ou obsolètes.</t>
+  </si>
+  <si>
+    <t>Administrateur Topnet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Presentation Du Rapport Suite au calcul </t>
+  </si>
+  <si>
+    <t>R-I-1</t>
+  </si>
+  <si>
+    <t>En tant qu'agent du Topnet, je peux générer et visualiser les rapports suite au calcul des critères d'engagement client, afin d'obtenir des informations détaillées sur les résultats de l'évaluation.</t>
+  </si>
+  <si>
+    <t>Historique Backup</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Rapport</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Backup</t>
+  </si>
+  <si>
+    <t>B-I-1</t>
+  </si>
+  <si>
+    <t>Statistique</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Voir Et Consultation De L'Evolution</t>
+  </si>
+  <si>
+    <t>S-I-1</t>
+  </si>
+  <si>
+    <t>En tant qu'agent du Topnet, je peux accéder aux statistiques relatives à l'évolution des indicateurs clés de performance (KPI) du système pour analyser les tendances et prendre des décisions éclairées.</t>
+  </si>
+  <si>
+    <t>Generation Une Simulation</t>
+  </si>
+  <si>
+    <t>Simulation</t>
+  </si>
+  <si>
+    <t>GS-I-1</t>
+  </si>
+  <si>
+    <t>En tant qu'agent du Topnet, je peux créer des simulations basées sur différents scénarios pour évaluer l'impact des changements potentiels sur les performances du système.</t>
+  </si>
+  <si>
+    <t>Configuration</t>
+  </si>
+  <si>
+    <t>Saisir Les Parametres Du Score</t>
+  </si>
+  <si>
+    <t>C-I-1</t>
+  </si>
+  <si>
+    <t>En tant qu'agent du Topnet, je peux configurer les paramètres utilisés pour établir les scores d'engagement client et de comportement client.</t>
+  </si>
+  <si>
+    <t>Stockage De Données</t>
+  </si>
+  <si>
+    <t>Saisir Les  Stockage Du Score</t>
+  </si>
+  <si>
+    <t>SDD-I-1</t>
+  </si>
+  <si>
+    <t>En tant qu'agent du Topnet, je peux gérer et stocker de manière sécurisée les données clients et les résultats d'évaluation dans le système.</t>
+  </si>
+  <si>
+    <t>Classemment Des Clients</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Categorie Client</t>
+  </si>
+  <si>
+    <t>En tant qu'agent du Topnet, je peux classer et catégoriser les clients en fonction de leur valeur commerciale, permettant un filtrage et un tri efficaces.</t>
+  </si>
+  <si>
+    <t>CCL-I-1</t>
+  </si>
+  <si>
+    <t>Générer un rapport pour une période spécifiée en utilisant les critères définis.
+Vérifier que le rapport présente les résultats d'évaluation de manière lisible et compréhensible.
+Vérifier que les informations fournies dans le rapport sont précises et à jour.</t>
+  </si>
+  <si>
+    <t>Générer des statistiques pour une période spécifiée en utilisant les critères d'offre définis.
+Présenter les statistiques sous forme de graphiques ou de tableaux faciles à comprendre.
+Permettre aux utilisateurs de consulter l'évolution des KPI sur différentes périodes pour analyser les tendances.</t>
+  </si>
+  <si>
+    <t>Définir les critères d'engagement client basés sur l'ancienneté, le montant de l'encours, le délai moyen de paiement, etc.
+Configurer les scores d'engagement client en attribuant des poids à chaque critère.
+Vérifier que les scores sont calculés de manière précise et cohérente pour chaque client.
+Appliquer les seuils de classification pour catégoriser les clients en fonction de leur valeur commerciale ou comportement.</t>
+  </si>
+  <si>
+    <t>Définir les paramètres de simulation, tels que le taux de croissance, le taux de conversion, les coûts opérationnels, etc.
+Créer une simulation en utilisant les paramètres spécifiés.
+Vérifier que les résultats des simulations sont présentés de manière claire et significative.
+Permettre aux utilisateurs de comparer les résultats des différentes simulations pour prendre des décisions éclairées.</t>
+  </si>
+  <si>
+    <t>Classer chaque client en fonction des critères de catégorisation spécifiés.
+Permettre aux utilisateurs de filtrer rapidement les clients dans des catégories spécifiques.
+Assurer que les données affichées sont cohérentes avec les résultats d'évaluation précédemment calculés.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> saisir les critères d'engagement client et de comportement client qui seront utilisés pour calculer les scores , spécifie les différents critères tels que l'ancienneté, le montant de l'encours, le délai moyen de paiement, etc.</t>
+  </si>
+  <si>
+    <t>Genere un historique pour les donnes Du Systéme</t>
+  </si>
+  <si>
+    <t>Adminstrateur Topnet</t>
+  </si>
+  <si>
+    <t>En tant qu'adminstrateur Du Topnet, Assurer la sauvegarde régulière et la gestion de l'historique des données du système.</t>
   </si>
 </sst>
 </file>
@@ -396,7 +546,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="32">
+  <fills count="29">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -513,18 +663,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor rgb="FFFFD966"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.249977111117893"/>
         <bgColor rgb="FFFFD966"/>
       </patternFill>
@@ -577,14 +715,8 @@
         <bgColor rgb="FF3C78D8"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.34998626667073579"/>
-        <bgColor rgb="FF3C78D8"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -775,11 +907,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -860,31 +1005,82 @@
     <xf numFmtId="0" fontId="10" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="24" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="25" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -893,123 +1089,48 @@
     <xf numFmtId="0" fontId="10" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="26" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="27" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="28" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1041,6 +1162,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="16" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1261,10 +1391,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -1300,29 +1430,29 @@
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E1" s="12" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="177" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="78" t="s">
+      <c r="A2" s="70" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="13"/>
@@ -1330,23 +1460,23 @@
         <v>3</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="G2" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" s="16" t="s">
         <v>46</v>
-      </c>
-      <c r="H2" s="16" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="154.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="79"/>
+      <c r="A3" s="71"/>
       <c r="B3" s="17">
         <v>1</v>
       </c>
@@ -1354,316 +1484,539 @@
         <v>4</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F3" s="19" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="G3" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3" s="20" t="s">
         <v>46</v>
-      </c>
-      <c r="H3" s="20" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="102.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="79"/>
+      <c r="A4" s="71"/>
       <c r="B4" s="21"/>
       <c r="C4" s="22" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="G4" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="H4" s="23" t="s">
         <v>46</v>
-      </c>
-      <c r="H4" s="23" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="105.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="80"/>
+      <c r="A5" s="72"/>
       <c r="B5" s="24"/>
       <c r="C5" s="25" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="E5" s="26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F5" s="26" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="G5" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" s="27" t="s">
         <v>46</v>
-      </c>
-      <c r="H5" s="27" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="138.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="81" t="s">
+      <c r="A6" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="28"/>
-      <c r="C6" s="29" t="s">
+      <c r="B6" s="83"/>
+      <c r="C6" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="30" t="s">
-        <v>70</v>
-      </c>
-      <c r="E6" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" s="31" t="s">
-        <v>55</v>
-      </c>
-      <c r="G6" s="31" t="s">
+      <c r="D6" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="E6" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="G6" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="H6" s="31" t="s">
         <v>46</v>
-      </c>
-      <c r="H6" s="32" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="123.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="82"/>
-      <c r="B7" s="33">
+      <c r="A7" s="74"/>
+      <c r="B7" s="32">
         <v>2</v>
       </c>
-      <c r="C7" s="34" t="s">
+      <c r="C7" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="35" t="s">
-        <v>71</v>
-      </c>
-      <c r="E7" s="36" t="s">
-        <v>34</v>
-      </c>
-      <c r="F7" s="36" t="s">
-        <v>60</v>
-      </c>
-      <c r="G7" s="36" t="s">
+      <c r="D7" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="E7" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="G7" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="H7" s="36" t="s">
         <v>46</v>
-      </c>
-      <c r="H7" s="37" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="171" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="83"/>
-      <c r="B8" s="38"/>
-      <c r="C8" s="39" t="s">
+      <c r="A8" s="75"/>
+      <c r="B8" s="37"/>
+      <c r="C8" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="40" t="s">
-        <v>72</v>
-      </c>
-      <c r="E8" s="41" t="s">
-        <v>35</v>
-      </c>
-      <c r="F8" s="41" t="s">
-        <v>56</v>
-      </c>
-      <c r="G8" s="41" t="s">
+      <c r="D8" s="39" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="H8" s="41" t="s">
         <v>46</v>
-      </c>
-      <c r="H8" s="42" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="138.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="84" t="s">
+      <c r="A9" s="76" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="43">
+      <c r="B9" s="82">
         <v>3</v>
       </c>
-      <c r="C9" s="44" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="45" t="s">
-        <v>73</v>
-      </c>
-      <c r="E9" s="46" t="s">
-        <v>36</v>
-      </c>
-      <c r="F9" s="46" t="s">
-        <v>57</v>
-      </c>
-      <c r="G9" s="46" t="s">
+      <c r="C9" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="43" t="s">
+        <v>68</v>
+      </c>
+      <c r="E9" s="44" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="G9" s="44" t="s">
+        <v>43</v>
+      </c>
+      <c r="H9" s="45" t="s">
         <v>46</v>
-      </c>
-      <c r="H9" s="47" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="234" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="85"/>
-      <c r="B10" s="48"/>
-      <c r="C10" s="49" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="50" t="s">
-        <v>74</v>
-      </c>
-      <c r="E10" s="51" t="s">
-        <v>37</v>
-      </c>
-      <c r="F10" s="51" t="s">
-        <v>58</v>
-      </c>
-      <c r="G10" s="51" t="s">
+      <c r="A10" s="77"/>
+      <c r="B10" s="46"/>
+      <c r="C10" s="47" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="48" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" s="49" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" s="49" t="s">
+        <v>54</v>
+      </c>
+      <c r="G10" s="49" t="s">
+        <v>43</v>
+      </c>
+      <c r="H10" s="50" t="s">
         <v>46</v>
-      </c>
-      <c r="H10" s="52" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="152.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="86" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="53"/>
-      <c r="C11" s="54" t="s">
+      <c r="A11" s="78" t="s">
+        <v>77</v>
+      </c>
+      <c r="B11" s="81"/>
+      <c r="C11" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="55" t="s">
-        <v>75</v>
-      </c>
-      <c r="E11" s="56" t="s">
-        <v>38</v>
-      </c>
-      <c r="F11" s="56" t="s">
-        <v>59</v>
-      </c>
-      <c r="G11" s="56" t="s">
+      <c r="D11" s="52" t="s">
+        <v>70</v>
+      </c>
+      <c r="E11" s="53" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="53" t="s">
+        <v>55</v>
+      </c>
+      <c r="G11" s="53" t="s">
+        <v>43</v>
+      </c>
+      <c r="H11" s="54" t="s">
         <v>46</v>
-      </c>
-      <c r="H11" s="57" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="166.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="87"/>
-      <c r="B12" s="58">
+      <c r="A12" s="79"/>
+      <c r="B12" s="55">
         <v>4</v>
       </c>
-      <c r="C12" s="59" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="60" t="s">
-        <v>76</v>
-      </c>
-      <c r="E12" s="61" t="s">
-        <v>39</v>
-      </c>
-      <c r="F12" s="61" t="s">
-        <v>53</v>
-      </c>
-      <c r="G12" s="61" t="s">
+      <c r="C12" s="56" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="57" t="s">
+        <v>71</v>
+      </c>
+      <c r="E12" s="58" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" s="58" t="s">
+        <v>49</v>
+      </c>
+      <c r="G12" s="58" t="s">
+        <v>43</v>
+      </c>
+      <c r="H12" s="59" t="s">
         <v>46</v>
-      </c>
-      <c r="H12" s="62" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="258" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="88"/>
-      <c r="B13" s="63"/>
-      <c r="C13" s="64" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="65" t="s">
-        <v>77</v>
-      </c>
-      <c r="E13" s="66" t="s">
-        <v>40</v>
-      </c>
-      <c r="F13" s="67" t="s">
-        <v>61</v>
-      </c>
-      <c r="G13" s="68" t="s">
+      <c r="A13" s="80"/>
+      <c r="B13" s="60"/>
+      <c r="C13" s="61" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="62" t="s">
+        <v>72</v>
+      </c>
+      <c r="E13" s="63" t="s">
+        <v>39</v>
+      </c>
+      <c r="F13" s="64" t="s">
+        <v>57</v>
+      </c>
+      <c r="G13" s="65" t="s">
+        <v>43</v>
+      </c>
+      <c r="H13" s="66" t="s">
         <v>46</v>
-      </c>
-      <c r="H13" s="69" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="301.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="70" t="s">
-        <v>42</v>
-      </c>
-      <c r="B14" s="71">
+      <c r="A14" s="67" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="69">
         <v>5</v>
       </c>
-      <c r="C14" s="72" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="72" t="s">
+      <c r="C14" s="68" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="68" t="s">
+        <v>73</v>
+      </c>
+      <c r="E14" s="68" t="s">
+        <v>40</v>
+      </c>
+      <c r="F14" s="68" t="s">
+        <v>58</v>
+      </c>
+      <c r="G14" s="68" t="s">
+        <v>43</v>
+      </c>
+      <c r="H14" s="69" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="156.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="78" t="s">
         <v>78</v>
       </c>
-      <c r="E14" s="72" t="s">
-        <v>41</v>
-      </c>
-      <c r="F14" s="72" t="s">
-        <v>62</v>
-      </c>
-      <c r="G14" s="72" t="s">
+      <c r="B15" s="81"/>
+      <c r="C15" s="51" t="s">
+        <v>79</v>
+      </c>
+      <c r="D15" s="52" t="s">
+        <v>82</v>
+      </c>
+      <c r="E15" s="53" t="s">
+        <v>85</v>
+      </c>
+      <c r="F15" s="53" t="s">
+        <v>86</v>
+      </c>
+      <c r="G15" s="53" t="s">
+        <v>43</v>
+      </c>
+      <c r="H15" s="54" t="s">
         <v>46</v>
       </c>
-      <c r="H14" s="73" t="s">
-        <v>51</v>
-      </c>
     </row>
-    <row r="15" spans="1:8" ht="213.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="74" t="s">
+    <row r="16" spans="1:8" ht="92.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A16" s="79"/>
+      <c r="B16" s="55">
+        <v>6</v>
+      </c>
+      <c r="C16" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="D16" s="57" t="s">
+        <v>83</v>
+      </c>
+      <c r="E16" s="58" t="s">
+        <v>87</v>
+      </c>
+      <c r="F16" s="58" t="s">
+        <v>88</v>
+      </c>
+      <c r="G16" s="58" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="75"/>
-      <c r="C15" s="76" t="s">
-        <v>44</v>
-      </c>
-      <c r="D15" s="76" t="s">
-        <v>79</v>
-      </c>
-      <c r="E15" s="76" t="s">
+      <c r="H16" s="59" t="s">
         <v>47</v>
       </c>
-      <c r="F15" s="76" t="s">
-        <v>63</v>
-      </c>
-      <c r="G15" s="76" t="s">
+    </row>
+    <row r="17" spans="1:8" ht="207" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A17" s="80"/>
+      <c r="B17" s="60"/>
+      <c r="C17" s="61" t="s">
+        <v>81</v>
+      </c>
+      <c r="D17" s="62" t="s">
+        <v>84</v>
+      </c>
+      <c r="E17" s="63" t="s">
+        <v>89</v>
+      </c>
+      <c r="F17" s="64" t="s">
+        <v>90</v>
+      </c>
+      <c r="G17" s="65" t="s">
+        <v>43</v>
+      </c>
+      <c r="H17" s="66" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="240" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A18" s="67" t="s">
+        <v>92</v>
+      </c>
+      <c r="B18" s="69">
+        <v>7</v>
+      </c>
+      <c r="C18" s="68" t="s">
+        <v>96</v>
+      </c>
+      <c r="D18" s="68" t="s">
+        <v>93</v>
+      </c>
+      <c r="E18" s="68" t="s">
+        <v>94</v>
+      </c>
+      <c r="F18" s="68" t="s">
+        <v>119</v>
+      </c>
+      <c r="G18" s="68" t="s">
+        <v>43</v>
+      </c>
+      <c r="H18" s="69" t="s">
         <v>46</v>
       </c>
-      <c r="H15" s="77" t="s">
-        <v>51</v>
-      </c>
     </row>
-    <row r="16" spans="1:8" ht="156.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="17" ht="92.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="18" ht="210.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="19" ht="96.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="20" ht="107.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="21" ht="177" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="22" ht="255" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="19" spans="1:8" ht="107.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A19" s="67" t="s">
+        <v>95</v>
+      </c>
+      <c r="B19" s="69">
+        <v>8</v>
+      </c>
+      <c r="C19" s="68" t="s">
+        <v>97</v>
+      </c>
+      <c r="D19" s="68" t="s">
+        <v>98</v>
+      </c>
+      <c r="E19" s="68" t="s">
+        <v>127</v>
+      </c>
+      <c r="F19" s="68" t="s">
+        <v>125</v>
+      </c>
+      <c r="G19" s="68" t="s">
+        <v>43</v>
+      </c>
+      <c r="H19" s="69" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="177" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A20" s="67" t="s">
+        <v>99</v>
+      </c>
+      <c r="B20" s="69">
+        <v>9</v>
+      </c>
+      <c r="C20" s="68" t="s">
+        <v>100</v>
+      </c>
+      <c r="D20" s="68" t="s">
+        <v>101</v>
+      </c>
+      <c r="E20" s="68" t="s">
+        <v>102</v>
+      </c>
+      <c r="F20" s="68" t="s">
+        <v>120</v>
+      </c>
+      <c r="G20" s="68" t="s">
+        <v>43</v>
+      </c>
+      <c r="H20" s="69" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="248.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A21" s="67" t="s">
+        <v>103</v>
+      </c>
+      <c r="B21" s="69">
+        <v>10</v>
+      </c>
+      <c r="C21" s="68" t="s">
+        <v>104</v>
+      </c>
+      <c r="D21" s="68" t="s">
+        <v>105</v>
+      </c>
+      <c r="E21" s="68" t="s">
+        <v>106</v>
+      </c>
+      <c r="F21" s="68" t="s">
+        <v>122</v>
+      </c>
+      <c r="G21" s="68" t="s">
+        <v>43</v>
+      </c>
+      <c r="H21" s="69" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="141.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A22" s="67" t="s">
+        <v>107</v>
+      </c>
+      <c r="B22" s="69">
+        <v>11</v>
+      </c>
+      <c r="C22" s="68" t="s">
+        <v>108</v>
+      </c>
+      <c r="D22" s="68" t="s">
+        <v>109</v>
+      </c>
+      <c r="E22" s="68" t="s">
+        <v>110</v>
+      </c>
+      <c r="F22" s="68" t="s">
+        <v>124</v>
+      </c>
+      <c r="G22" s="68" t="s">
+        <v>43</v>
+      </c>
+      <c r="H22" s="69" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="149.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A23" s="67" t="s">
+        <v>111</v>
+      </c>
+      <c r="B23" s="69">
+        <v>12</v>
+      </c>
+      <c r="C23" s="68" t="s">
+        <v>112</v>
+      </c>
+      <c r="D23" s="68" t="s">
+        <v>113</v>
+      </c>
+      <c r="E23" s="68" t="s">
+        <v>114</v>
+      </c>
+      <c r="F23" s="68" t="s">
+        <v>121</v>
+      </c>
+      <c r="G23" s="68" t="s">
+        <v>43</v>
+      </c>
+      <c r="H23" s="69" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A24" s="67" t="s">
+        <v>115</v>
+      </c>
+      <c r="B24" s="69">
+        <v>13</v>
+      </c>
+      <c r="C24" s="68" t="s">
+        <v>116</v>
+      </c>
+      <c r="D24" s="68" t="s">
+        <v>118</v>
+      </c>
+      <c r="E24" s="68" t="s">
+        <v>117</v>
+      </c>
+      <c r="F24" s="68" t="s">
+        <v>123</v>
+      </c>
+      <c r="G24" s="68" t="s">
+        <v>43</v>
+      </c>
+      <c r="H24" s="69" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="75.75" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A15:A17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1691,7 +2044,7 @@
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="1"/>
@@ -1721,7 +2074,7 @@
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="1"/>
@@ -1751,7 +2104,7 @@
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="1"/>
@@ -1781,7 +2134,7 @@
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="1"/>
@@ -2839,33 +3192,33 @@
   <sheetData>
     <row r="2" spans="1:26" ht="23.25" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>

</xml_diff>

<commit_message>
Maj Sprint Backlog / Journal
Co-Authored-By: Nacib Mariem <67750731+Nacib1999@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Conception Du Projet/TOPNET-Sprint Backlog scoring.xlsx
+++ b/Conception Du Projet/TOPNET-Sprint Backlog scoring.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Topnet-B2C-Stage-\Conception Du Projet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6C52DFB-3750-40B4-8C6A-282765969426}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B581D9C-1162-4AFF-8D1E-8158B97EE66F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="117">
   <si>
     <t>Theme</t>
   </si>
@@ -160,13 +160,7 @@
     <t xml:space="preserve">A Faire </t>
   </si>
   <si>
-    <t xml:space="preserve">                    Niveau Utilisateur</t>
-  </si>
-  <si>
     <t>Sprint</t>
-  </si>
-  <si>
-    <t>Agent Topnet</t>
   </si>
   <si>
     <t>Story Test</t>
@@ -290,9 +284,6 @@
     <t>• Je veux pouvoir créer de nouveaux comptes d'utilisateurs en fournissant les informations nécessaires (nom, rôle, mot de passe, etc.).
 • Je souhaite pouvoir modifier les informations des comptes existants, tels que les rôles ou les autorisations.
 • Je veux pouvoir supprimer des comptes d'utilisateurs non nécessaires ou obsolètes.</t>
-  </si>
-  <si>
-    <t>Administrateur Topnet</t>
   </si>
   <si>
     <t xml:space="preserve">Presentation Du Rapport Suite au calcul </t>
@@ -409,13 +400,19 @@
     <t>Genere un historique pour les donnes Du Systéme</t>
   </si>
   <si>
-    <t>Adminstrateur Topnet</t>
-  </si>
-  <si>
     <t>En tant qu'adminstrateur Du Topnet, je peux Assurer la sauvegarde régulière et la gestion de l'historique des données du système.</t>
   </si>
   <si>
     <t>Comportement client</t>
+  </si>
+  <si>
+    <t>Termine</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Termine </t>
   </si>
 </sst>
 </file>
@@ -642,7 +639,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -798,21 +795,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top/>
       <bottom style="thin">
@@ -924,11 +906,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -949,7 +970,7 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -970,9 +991,6 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -982,9 +1000,6 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -994,9 +1009,6 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1006,10 +1018,7 @@
     <xf numFmtId="0" fontId="7" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1021,9 +1030,6 @@
     <xf numFmtId="0" fontId="7" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1042,7 +1048,7 @@
     <xf numFmtId="0" fontId="7" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1054,9 +1060,6 @@
     <xf numFmtId="0" fontId="7" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1069,10 +1072,7 @@
     <xf numFmtId="0" fontId="7" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1105,64 +1105,137 @@
     <xf numFmtId="0" fontId="7" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="20" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="21" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="20" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1383,10 +1456,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="53" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="37" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -1398,53 +1471,49 @@
     <col min="5" max="5" width="202" style="6" customWidth="1"/>
     <col min="6" max="6" width="228.5703125" style="6" customWidth="1"/>
     <col min="7" max="7" width="172.7109375" style="6" customWidth="1"/>
-    <col min="8" max="8" width="87.140625" style="6" customWidth="1"/>
-    <col min="9" max="9" width="74" style="6" customWidth="1"/>
-    <col min="10" max="10" width="61.28515625" style="6" customWidth="1"/>
-    <col min="11" max="11" width="75.5703125" style="6" customWidth="1"/>
-    <col min="12" max="12" width="82.7109375" style="6" customWidth="1"/>
-    <col min="13" max="13" width="66.85546875" style="6" customWidth="1"/>
-    <col min="14" max="14" width="68.28515625" style="6" customWidth="1"/>
-    <col min="15" max="15" width="87.7109375" style="6" customWidth="1"/>
-    <col min="16" max="16" width="43.140625" style="6" customWidth="1"/>
-    <col min="17" max="17" width="50.28515625" style="6" customWidth="1"/>
-    <col min="18" max="18" width="40.28515625" style="6" customWidth="1"/>
-    <col min="19" max="19" width="44.85546875" style="6" customWidth="1"/>
-    <col min="20" max="20" width="33.140625" style="6" customWidth="1"/>
-    <col min="21" max="21" width="36.5703125" style="6" customWidth="1"/>
-    <col min="22" max="22" width="38.7109375" style="6" customWidth="1"/>
-    <col min="23" max="23" width="41.85546875" style="6" customWidth="1"/>
-    <col min="24" max="16384" width="14.42578125" style="6"/>
+    <col min="8" max="8" width="74" style="6" customWidth="1"/>
+    <col min="9" max="9" width="61.28515625" style="6" customWidth="1"/>
+    <col min="10" max="10" width="75.5703125" style="6" customWidth="1"/>
+    <col min="11" max="11" width="82.7109375" style="6" customWidth="1"/>
+    <col min="12" max="12" width="66.85546875" style="6" customWidth="1"/>
+    <col min="13" max="13" width="68.28515625" style="6" customWidth="1"/>
+    <col min="14" max="14" width="87.7109375" style="6" customWidth="1"/>
+    <col min="15" max="15" width="43.140625" style="6" customWidth="1"/>
+    <col min="16" max="16" width="50.28515625" style="6" customWidth="1"/>
+    <col min="17" max="17" width="40.28515625" style="6" customWidth="1"/>
+    <col min="18" max="18" width="44.85546875" style="6" customWidth="1"/>
+    <col min="19" max="19" width="33.140625" style="6" customWidth="1"/>
+    <col min="20" max="20" width="36.5703125" style="6" customWidth="1"/>
+    <col min="21" max="21" width="38.7109375" style="6" customWidth="1"/>
+    <col min="22" max="22" width="41.85546875" style="6" customWidth="1"/>
+    <col min="23" max="16384" width="14.42578125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" ht="60.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E1" s="11" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G1" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="H1" s="8" t="s">
-        <v>41</v>
-      </c>
     </row>
-    <row r="2" spans="1:8" ht="177" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="68" t="s">
+    <row r="2" spans="1:7" ht="177" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="61" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="12"/>
@@ -1452,498 +1521,411 @@
         <v>3</v>
       </c>
       <c r="D2" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" s="78" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="G2" s="73" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="154.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="62"/>
+      <c r="B3" s="15">
+        <v>1</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="72" t="s">
+        <v>66</v>
+      </c>
+      <c r="G3" s="77"/>
+    </row>
+    <row r="4" spans="1:7" ht="102.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="62"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="E2" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="G2" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="H2" s="15" t="s">
-        <v>43</v>
-      </c>
+      <c r="E4" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="74" t="s">
+        <v>44</v>
+      </c>
+      <c r="G4" s="79"/>
     </row>
-    <row r="3" spans="1:8" ht="154.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="69"/>
-      <c r="B3" s="16">
-        <v>1</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="17" t="s">
+    <row r="5" spans="1:7" ht="105.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="63"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="E3" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" s="18" t="s">
+      <c r="E5" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="75" t="s">
         <v>68</v>
       </c>
-      <c r="G3" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="H3" s="19" t="s">
-        <v>43</v>
-      </c>
+      <c r="G5" s="80"/>
     </row>
-    <row r="4" spans="1:8" ht="102.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="69"/>
-      <c r="B4" s="20"/>
-      <c r="C4" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="21" t="s">
+    <row r="6" spans="1:7" ht="138.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="64" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="24"/>
+      <c r="C6" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="E4" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="F4" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="G4" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="H4" s="23" t="s">
-        <v>43</v>
-      </c>
+      <c r="E6" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="76" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" s="81"/>
     </row>
-    <row r="5" spans="1:8" ht="105.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="70"/>
-      <c r="B5" s="24"/>
-      <c r="C5" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="E5" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" s="26" t="s">
-        <v>70</v>
-      </c>
-      <c r="G5" s="26" t="s">
-        <v>40</v>
-      </c>
-      <c r="H5" s="27" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="138.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="71" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="28"/>
-      <c r="C6" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="30" t="s">
-        <v>60</v>
-      </c>
-      <c r="E6" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" s="31" t="s">
-        <v>47</v>
-      </c>
-      <c r="G6" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="H6" s="32" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="123.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="72"/>
+    <row r="7" spans="1:7" ht="123.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="65"/>
       <c r="B7" s="12">
         <v>2</v>
       </c>
-      <c r="C7" s="33" t="s">
+      <c r="C7" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="34" t="s">
+      <c r="D7" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="E7" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="G7" s="83" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="171" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="66"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" s="82" t="s">
+        <v>46</v>
+      </c>
+      <c r="G8" s="85"/>
+    </row>
+    <row r="9" spans="1:7" ht="138.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="67" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="34">
+        <v>3</v>
+      </c>
+      <c r="C9" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="E7" s="35" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" s="35" t="s">
-        <v>52</v>
-      </c>
-      <c r="G7" s="35" t="s">
+      <c r="E9" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" s="84" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" s="87" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="234" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="68"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="40" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" s="41" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" s="86" t="s">
+        <v>48</v>
+      </c>
+      <c r="G10" s="88"/>
+    </row>
+    <row r="11" spans="1:7" ht="152.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="69" t="s">
+        <v>113</v>
+      </c>
+      <c r="B11" s="42"/>
+      <c r="C11" s="43" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="44" t="s">
+        <v>63</v>
+      </c>
+      <c r="E11" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" s="45" t="s">
+        <v>49</v>
+      </c>
+      <c r="G11" s="90" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="166.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="70"/>
+      <c r="B12" s="21">
+        <v>4</v>
+      </c>
+      <c r="C12" s="46" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="47" t="s">
+        <v>64</v>
+      </c>
+      <c r="E12" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12" s="89" t="s">
+        <v>43</v>
+      </c>
+      <c r="G12" s="91"/>
+    </row>
+    <row r="13" spans="1:7" ht="258" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="71"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="60" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="60" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13" s="51" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" s="52" t="s">
+        <v>51</v>
+      </c>
+      <c r="G13" s="92"/>
+    </row>
+    <row r="14" spans="1:7" ht="156.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A14" s="69" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14" s="42"/>
+      <c r="C14" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="D14" s="44" t="s">
+        <v>72</v>
+      </c>
+      <c r="E14" s="93" t="s">
+        <v>74</v>
+      </c>
+      <c r="F14" s="93" t="s">
+        <v>75</v>
+      </c>
+      <c r="G14" s="94" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="207" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="71"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="49" t="s">
+        <v>71</v>
+      </c>
+      <c r="D15" s="50" t="s">
+        <v>73</v>
+      </c>
+      <c r="E15" s="51" t="s">
+        <v>76</v>
+      </c>
+      <c r="F15" s="52" t="s">
+        <v>77</v>
+      </c>
+      <c r="G15" s="95"/>
+    </row>
+    <row r="16" spans="1:7" ht="240" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A16" s="54" t="s">
+        <v>78</v>
+      </c>
+      <c r="B16" s="57">
+        <v>6</v>
+      </c>
+      <c r="C16" s="53" t="s">
+        <v>82</v>
+      </c>
+      <c r="D16" s="53" t="s">
+        <v>79</v>
+      </c>
+      <c r="E16" s="53" t="s">
+        <v>80</v>
+      </c>
+      <c r="F16" s="53" t="s">
+        <v>105</v>
+      </c>
+      <c r="G16" s="95" t="s">
         <v>40</v>
       </c>
-      <c r="H7" s="15" t="s">
-        <v>43</v>
-      </c>
     </row>
-    <row r="8" spans="1:8" ht="171" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="73"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="36" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="37" t="s">
-        <v>62</v>
-      </c>
-      <c r="E8" s="38" t="s">
-        <v>33</v>
-      </c>
-      <c r="F8" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="G8" s="38" t="s">
+    <row r="17" spans="1:7" ht="107.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A17" s="55" t="s">
+        <v>81</v>
+      </c>
+      <c r="B17" s="57">
+        <v>7</v>
+      </c>
+      <c r="C17" s="56" t="s">
+        <v>83</v>
+      </c>
+      <c r="D17" s="53" t="s">
+        <v>84</v>
+      </c>
+      <c r="E17" s="53" t="s">
+        <v>112</v>
+      </c>
+      <c r="F17" s="53" t="s">
+        <v>111</v>
+      </c>
+      <c r="G17" s="97" t="s">
         <v>40</v>
       </c>
-      <c r="H8" s="19" t="s">
-        <v>43</v>
-      </c>
     </row>
-    <row r="9" spans="1:8" ht="138.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="74" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="39">
-        <v>3</v>
-      </c>
-      <c r="C9" s="40" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="41" t="s">
-        <v>63</v>
-      </c>
-      <c r="E9" s="42" t="s">
-        <v>34</v>
-      </c>
-      <c r="F9" s="42" t="s">
-        <v>49</v>
-      </c>
-      <c r="G9" s="42" t="s">
+    <row r="18" spans="1:7" ht="177" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A18" s="54" t="s">
+        <v>85</v>
+      </c>
+      <c r="B18" s="59"/>
+      <c r="C18" s="53" t="s">
+        <v>86</v>
+      </c>
+      <c r="D18" s="53" t="s">
+        <v>87</v>
+      </c>
+      <c r="E18" s="53" t="s">
+        <v>88</v>
+      </c>
+      <c r="F18" s="96" t="s">
+        <v>106</v>
+      </c>
+      <c r="G18" s="91"/>
+    </row>
+    <row r="19" spans="1:7" ht="248.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A19" s="55" t="s">
+        <v>89</v>
+      </c>
+      <c r="B19" s="59"/>
+      <c r="C19" s="56" t="s">
+        <v>90</v>
+      </c>
+      <c r="D19" s="53" t="s">
+        <v>91</v>
+      </c>
+      <c r="E19" s="53" t="s">
+        <v>92</v>
+      </c>
+      <c r="F19" s="96" t="s">
+        <v>108</v>
+      </c>
+      <c r="G19" s="91"/>
+    </row>
+    <row r="20" spans="1:7" ht="141.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A20" s="54" t="s">
+        <v>93</v>
+      </c>
+      <c r="B20" s="58"/>
+      <c r="C20" s="53" t="s">
+        <v>94</v>
+      </c>
+      <c r="D20" s="53" t="s">
+        <v>95</v>
+      </c>
+      <c r="E20" s="53" t="s">
+        <v>96</v>
+      </c>
+      <c r="F20" s="96" t="s">
+        <v>110</v>
+      </c>
+      <c r="G20" s="91"/>
+    </row>
+    <row r="21" spans="1:7" ht="149.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A21" s="54" t="s">
+        <v>97</v>
+      </c>
+      <c r="B21" s="57">
+        <v>8</v>
+      </c>
+      <c r="C21" s="53" t="s">
+        <v>98</v>
+      </c>
+      <c r="D21" s="53" t="s">
+        <v>99</v>
+      </c>
+      <c r="E21" s="53" t="s">
+        <v>100</v>
+      </c>
+      <c r="F21" s="53" t="s">
+        <v>107</v>
+      </c>
+      <c r="G21" s="95" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="105" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A22" s="55" t="s">
+        <v>101</v>
+      </c>
+      <c r="B22" s="58"/>
+      <c r="C22" s="56" t="s">
+        <v>102</v>
+      </c>
+      <c r="D22" s="53" t="s">
+        <v>104</v>
+      </c>
+      <c r="E22" s="53" t="s">
+        <v>103</v>
+      </c>
+      <c r="F22" s="53" t="s">
+        <v>109</v>
+      </c>
+      <c r="G22" s="53" t="s">
         <v>40</v>
       </c>
-      <c r="H9" s="43" t="s">
-        <v>43</v>
-      </c>
     </row>
-    <row r="10" spans="1:8" ht="234" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="75"/>
-      <c r="B10" s="44"/>
-      <c r="C10" s="45" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="46" t="s">
-        <v>64</v>
-      </c>
-      <c r="E10" s="47" t="s">
-        <v>35</v>
-      </c>
-      <c r="F10" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="G10" s="47" t="s">
-        <v>40</v>
-      </c>
-      <c r="H10" s="48" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="152.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="76" t="s">
-        <v>117</v>
-      </c>
-      <c r="B11" s="49"/>
-      <c r="C11" s="50" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="51" t="s">
-        <v>65</v>
-      </c>
-      <c r="E11" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="F11" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="G11" s="52" t="s">
-        <v>40</v>
-      </c>
-      <c r="H11" s="27" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="166.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="77"/>
-      <c r="B12" s="24">
-        <v>4</v>
-      </c>
-      <c r="C12" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="54" t="s">
-        <v>66</v>
-      </c>
-      <c r="E12" s="55" t="s">
-        <v>37</v>
-      </c>
-      <c r="F12" s="55" t="s">
-        <v>45</v>
-      </c>
-      <c r="G12" s="55" t="s">
-        <v>40</v>
-      </c>
-      <c r="H12" s="27" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="258" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="78"/>
-      <c r="B13" s="24"/>
-      <c r="C13" s="79" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="79" t="s">
-        <v>67</v>
-      </c>
-      <c r="E13" s="58" t="s">
-        <v>38</v>
-      </c>
-      <c r="F13" s="59" t="s">
-        <v>53</v>
-      </c>
-      <c r="G13" s="60" t="s">
-        <v>40</v>
-      </c>
-      <c r="H13" s="27" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="156.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="76" t="s">
-        <v>71</v>
-      </c>
-      <c r="B14" s="49"/>
-      <c r="C14" s="50" t="s">
-        <v>72</v>
-      </c>
-      <c r="D14" s="51" t="s">
-        <v>74</v>
-      </c>
-      <c r="E14" s="52" t="s">
-        <v>76</v>
-      </c>
-      <c r="F14" s="52" t="s">
-        <v>77</v>
-      </c>
-      <c r="G14" s="52" t="s">
-        <v>40</v>
-      </c>
-      <c r="H14" s="27" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="207" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="78"/>
-      <c r="B15" s="24"/>
-      <c r="C15" s="56" t="s">
-        <v>73</v>
-      </c>
-      <c r="D15" s="57" t="s">
-        <v>75</v>
-      </c>
-      <c r="E15" s="58" t="s">
-        <v>78</v>
-      </c>
-      <c r="F15" s="59" t="s">
-        <v>79</v>
-      </c>
-      <c r="G15" s="60" t="s">
-        <v>40</v>
-      </c>
-      <c r="H15" s="27" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="240" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="62" t="s">
-        <v>81</v>
-      </c>
-      <c r="B16" s="65">
-        <v>6</v>
-      </c>
-      <c r="C16" s="61" t="s">
-        <v>85</v>
-      </c>
-      <c r="D16" s="61" t="s">
-        <v>82</v>
-      </c>
-      <c r="E16" s="61" t="s">
-        <v>83</v>
-      </c>
-      <c r="F16" s="61" t="s">
-        <v>108</v>
-      </c>
-      <c r="G16" s="61" t="s">
-        <v>40</v>
-      </c>
-      <c r="H16" s="27" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="107.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="63" t="s">
-        <v>84</v>
-      </c>
-      <c r="B17" s="65">
-        <v>7</v>
-      </c>
-      <c r="C17" s="64" t="s">
-        <v>86</v>
-      </c>
-      <c r="D17" s="61" t="s">
-        <v>87</v>
-      </c>
-      <c r="E17" s="61" t="s">
-        <v>116</v>
-      </c>
-      <c r="F17" s="61" t="s">
-        <v>114</v>
-      </c>
-      <c r="G17" s="61" t="s">
-        <v>40</v>
-      </c>
-      <c r="H17" s="27" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="177" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="62" t="s">
-        <v>88</v>
-      </c>
-      <c r="B18" s="67"/>
-      <c r="C18" s="61" t="s">
-        <v>89</v>
-      </c>
-      <c r="D18" s="61" t="s">
-        <v>90</v>
-      </c>
-      <c r="E18" s="61" t="s">
-        <v>91</v>
-      </c>
-      <c r="F18" s="61" t="s">
-        <v>109</v>
-      </c>
-      <c r="G18" s="61" t="s">
-        <v>40</v>
-      </c>
-      <c r="H18" s="27" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="248.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A19" s="63" t="s">
-        <v>92</v>
-      </c>
-      <c r="B19" s="67"/>
-      <c r="C19" s="64" t="s">
-        <v>93</v>
-      </c>
-      <c r="D19" s="61" t="s">
-        <v>94</v>
-      </c>
-      <c r="E19" s="61" t="s">
-        <v>95</v>
-      </c>
-      <c r="F19" s="61" t="s">
-        <v>111</v>
-      </c>
-      <c r="G19" s="61" t="s">
-        <v>40</v>
-      </c>
-      <c r="H19" s="27" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="141.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="62" t="s">
-        <v>96</v>
-      </c>
-      <c r="B20" s="66"/>
-      <c r="C20" s="61" t="s">
-        <v>97</v>
-      </c>
-      <c r="D20" s="61" t="s">
-        <v>98</v>
-      </c>
-      <c r="E20" s="61" t="s">
-        <v>99</v>
-      </c>
-      <c r="F20" s="61" t="s">
-        <v>113</v>
-      </c>
-      <c r="G20" s="61" t="s">
-        <v>40</v>
-      </c>
-      <c r="H20" s="27" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="149.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="62" t="s">
-        <v>100</v>
-      </c>
-      <c r="B21" s="65">
-        <v>8</v>
-      </c>
-      <c r="C21" s="61" t="s">
-        <v>101</v>
-      </c>
-      <c r="D21" s="61" t="s">
-        <v>102</v>
-      </c>
-      <c r="E21" s="61" t="s">
-        <v>103</v>
-      </c>
-      <c r="F21" s="61" t="s">
-        <v>110</v>
-      </c>
-      <c r="G21" s="61" t="s">
-        <v>40</v>
-      </c>
-      <c r="H21" s="27" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="63" t="s">
-        <v>104</v>
-      </c>
-      <c r="B22" s="66"/>
-      <c r="C22" s="64" t="s">
-        <v>105</v>
-      </c>
-      <c r="D22" s="61" t="s">
-        <v>107</v>
-      </c>
-      <c r="E22" s="61" t="s">
-        <v>106</v>
-      </c>
-      <c r="F22" s="61" t="s">
-        <v>112</v>
-      </c>
-      <c r="G22" s="61" t="s">
-        <v>40</v>
-      </c>
-      <c r="H22" s="27" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="75.75" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="23" spans="1:7" ht="75.75" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A2:A5"/>

</xml_diff>

<commit_message>
Update Journal / Sprint Backlog / Optimisation Du Code
Co-Authored-By: Nacib Mariem <67750731+Nacib1999@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Conception Du Projet/TOPNET-Sprint Backlog scoring.xlsx
+++ b/Conception Du Projet/TOPNET-Sprint Backlog scoring.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Topnet-B2C-Stage-\Conception Du Projet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81F15F9A-F479-4810-B093-9DE3CA4D2715}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2E9533F-365E-47DD-8808-A675161112CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="109">
   <si>
     <t>Theme</t>
   </si>
@@ -383,9 +383,6 @@
   </si>
   <si>
     <t xml:space="preserve">Termine </t>
-  </si>
-  <si>
-    <t>En Cours</t>
   </si>
   <si>
     <t xml:space="preserve"> Rapport  </t>
@@ -490,7 +487,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="22">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -511,110 +508,188 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="8"/>
         <bgColor rgb="FF0B5394"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="8"/>
         <bgColor rgb="FFC9DAF8"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="8"/>
         <bgColor rgb="FFA4C2F4"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="8"/>
         <bgColor rgb="FF6D9EEB"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="8"/>
         <bgColor rgb="FF3C78D8"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor rgb="FF6AA84F"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor rgb="FF980000"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor rgb="FFD9EAD3"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor rgb="FFC9DAF8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor rgb="FFB6D7A8"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor rgb="FF93C47D"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor rgb="FFA4C2F4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor rgb="FFA64D79"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor rgb="FFEAD1DC"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor rgb="FFD5A6BD"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor rgb="FFF1C232"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor rgb="FF3C78D8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor rgb="FFFFF2CC"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor rgb="FFFFE599"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor rgb="FFFFD966"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor rgb="FFF1C232"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor rgb="FF3C78D8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor rgb="FFFFF2CC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor rgb="FFFFD966"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor rgb="FF3C78D8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor rgb="FFFFD966"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor rgb="FF3C78D8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor rgb="FFFFD966"/>
       </patternFill>
     </fill>
   </fills>
@@ -928,7 +1003,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -961,15 +1036,27 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -979,6 +1066,12 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -988,6 +1081,15 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -997,6 +1099,15 @@
     <xf numFmtId="0" fontId="7" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1009,49 +1120,76 @@
     <xf numFmtId="0" fontId="7" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1063,158 +1201,164 @@
     <xf numFmtId="0" fontId="7" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1437,8 +1581,8 @@
   </sheetPr>
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C17" zoomScale="62" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="62" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -1492,396 +1636,396 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="177" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="87" t="s">
+      <c r="A2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="13" t="s">
+      <c r="B2" s="13"/>
+      <c r="C2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="E2" s="67" t="s">
+      <c r="E2" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="G2" s="62" t="s">
+      <c r="G2" s="17" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="154.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="88"/>
-      <c r="B3" s="15">
+      <c r="A3" s="18"/>
+      <c r="B3" s="19">
         <v>1</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="61" t="s">
+      <c r="F3" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="G3" s="66"/>
+      <c r="G3" s="23"/>
     </row>
     <row r="4" spans="1:7" ht="102.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="88"/>
-      <c r="B4" s="18"/>
-      <c r="C4" s="19" t="s">
+      <c r="A4" s="18"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="E4" s="20" t="s">
+      <c r="E4" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="F4" s="63" t="s">
+      <c r="F4" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="G4" s="68"/>
+      <c r="G4" s="28"/>
     </row>
     <row r="5" spans="1:7" ht="105.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="89"/>
-      <c r="B5" s="21"/>
-      <c r="C5" s="22" t="s">
+      <c r="A5" s="29"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="E5" s="23" t="s">
+      <c r="E5" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="64" t="s">
+      <c r="F5" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="G5" s="69"/>
+      <c r="G5" s="34"/>
     </row>
     <row r="6" spans="1:7" ht="138.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="90" t="s">
+      <c r="A6" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="24"/>
-      <c r="C6" s="25" t="s">
+      <c r="B6" s="36"/>
+      <c r="C6" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="26" t="s">
+      <c r="D6" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="E6" s="27" t="s">
+      <c r="E6" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="65" t="s">
+      <c r="F6" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="G6" s="70"/>
+      <c r="G6" s="41"/>
     </row>
     <row r="7" spans="1:7" ht="123.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="91"/>
-      <c r="B7" s="12">
+      <c r="A7" s="42"/>
+      <c r="B7" s="43">
         <v>2</v>
       </c>
-      <c r="C7" s="28" t="s">
+      <c r="C7" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="29" t="s">
+      <c r="D7" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="E7" s="30" t="s">
+      <c r="E7" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="30" t="s">
+      <c r="F7" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="G7" s="72" t="s">
+      <c r="G7" s="47" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="171" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="92"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="31" t="s">
+      <c r="A8" s="48"/>
+      <c r="B8" s="49"/>
+      <c r="C8" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="32" t="s">
+      <c r="D8" s="51" t="s">
         <v>59</v>
       </c>
-      <c r="E8" s="33" t="s">
+      <c r="E8" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="F8" s="71" t="s">
+      <c r="F8" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="G8" s="74"/>
+      <c r="G8" s="54"/>
     </row>
     <row r="9" spans="1:7" ht="138.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="93" t="s">
+      <c r="A9" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="34">
+      <c r="B9" s="56">
         <v>3</v>
       </c>
-      <c r="C9" s="35" t="s">
+      <c r="C9" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="36" t="s">
+      <c r="D9" s="58" t="s">
         <v>60</v>
       </c>
-      <c r="E9" s="37" t="s">
+      <c r="E9" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="F9" s="73" t="s">
+      <c r="F9" s="60" t="s">
         <v>46</v>
       </c>
-      <c r="G9" s="76" t="s">
+      <c r="G9" s="61" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="234" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="94"/>
-      <c r="B10" s="38"/>
-      <c r="C10" s="39" t="s">
+      <c r="A10" s="62"/>
+      <c r="B10" s="63"/>
+      <c r="C10" s="64" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="40" t="s">
+      <c r="D10" s="65" t="s">
         <v>61</v>
       </c>
-      <c r="E10" s="41" t="s">
+      <c r="E10" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="F10" s="75" t="s">
+      <c r="F10" s="67" t="s">
         <v>47</v>
       </c>
-      <c r="G10" s="77"/>
+      <c r="G10" s="68"/>
     </row>
     <row r="11" spans="1:7" ht="152.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="95" t="s">
+      <c r="A11" s="69" t="s">
         <v>104</v>
       </c>
-      <c r="B11" s="42"/>
-      <c r="C11" s="43" t="s">
+      <c r="B11" s="70"/>
+      <c r="C11" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="44" t="s">
+      <c r="D11" s="72" t="s">
         <v>62</v>
       </c>
-      <c r="E11" s="45" t="s">
+      <c r="E11" s="73" t="s">
         <v>36</v>
       </c>
-      <c r="F11" s="45" t="s">
+      <c r="F11" s="73" t="s">
         <v>48</v>
       </c>
-      <c r="G11" s="79" t="s">
+      <c r="G11" s="74" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="166.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="96"/>
-      <c r="B12" s="21">
+      <c r="A12" s="75"/>
+      <c r="B12" s="76">
         <v>4</v>
       </c>
-      <c r="C12" s="46" t="s">
+      <c r="C12" s="77" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="47" t="s">
+      <c r="D12" s="78" t="s">
         <v>63</v>
       </c>
-      <c r="E12" s="48" t="s">
+      <c r="E12" s="79" t="s">
         <v>37</v>
       </c>
-      <c r="F12" s="78" t="s">
+      <c r="F12" s="80" t="s">
         <v>42</v>
       </c>
-      <c r="G12" s="80"/>
+      <c r="G12" s="81"/>
     </row>
     <row r="13" spans="1:7" ht="258" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="97"/>
-      <c r="B13" s="21"/>
-      <c r="C13" s="60" t="s">
+      <c r="A13" s="82"/>
+      <c r="B13" s="76"/>
+      <c r="C13" s="83" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="60" t="s">
+      <c r="D13" s="83" t="s">
         <v>64</v>
       </c>
-      <c r="E13" s="51" t="s">
+      <c r="E13" s="84" t="s">
         <v>38</v>
       </c>
-      <c r="F13" s="52" t="s">
+      <c r="F13" s="85" t="s">
         <v>50</v>
       </c>
-      <c r="G13" s="81"/>
+      <c r="G13" s="86"/>
     </row>
     <row r="14" spans="1:7" ht="156.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="95" t="s">
+      <c r="A14" s="87" t="s">
         <v>68</v>
       </c>
-      <c r="B14" s="42">
+      <c r="B14" s="88">
         <v>5</v>
       </c>
-      <c r="C14" s="43" t="s">
+      <c r="C14" s="89" t="s">
         <v>69</v>
       </c>
-      <c r="D14" s="44" t="s">
+      <c r="D14" s="90" t="s">
         <v>71</v>
       </c>
-      <c r="E14" s="82" t="s">
+      <c r="E14" s="91" t="s">
         <v>73</v>
       </c>
-      <c r="F14" s="82" t="s">
+      <c r="F14" s="91" t="s">
         <v>74</v>
       </c>
-      <c r="G14" s="83" t="s">
+      <c r="G14" s="92" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="207" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="97"/>
-      <c r="B15" s="21"/>
-      <c r="C15" s="49" t="s">
+      <c r="A15" s="93"/>
+      <c r="B15" s="94"/>
+      <c r="C15" s="95" t="s">
         <v>70</v>
       </c>
-      <c r="D15" s="50" t="s">
+      <c r="D15" s="96" t="s">
         <v>72</v>
       </c>
-      <c r="E15" s="51" t="s">
+      <c r="E15" s="97" t="s">
         <v>75</v>
       </c>
-      <c r="F15" s="52" t="s">
+      <c r="F15" s="98" t="s">
         <v>76</v>
       </c>
-      <c r="G15" s="84"/>
+      <c r="G15" s="99"/>
     </row>
     <row r="16" spans="1:7" ht="240" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="55" t="s">
+      <c r="A16" s="100" t="s">
         <v>91</v>
       </c>
-      <c r="B16" s="57">
+      <c r="B16" s="108">
         <v>6</v>
       </c>
-      <c r="C16" s="56" t="s">
+      <c r="C16" s="102" t="s">
         <v>92</v>
       </c>
-      <c r="D16" s="53" t="s">
+      <c r="D16" s="103" t="s">
         <v>93</v>
       </c>
-      <c r="E16" s="53" t="s">
+      <c r="E16" s="103" t="s">
         <v>94</v>
       </c>
-      <c r="F16" s="53" t="s">
+      <c r="F16" s="103" t="s">
         <v>100</v>
       </c>
-      <c r="G16" s="80" t="s">
+      <c r="G16" s="105" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="240" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="55" t="s">
+      <c r="A17" s="100" t="s">
         <v>83</v>
       </c>
-      <c r="B17" s="59"/>
-      <c r="C17" s="56" t="s">
+      <c r="B17" s="101"/>
+      <c r="C17" s="102" t="s">
         <v>84</v>
       </c>
-      <c r="D17" s="53" t="s">
+      <c r="D17" s="103" t="s">
         <v>85</v>
       </c>
-      <c r="E17" s="53" t="s">
+      <c r="E17" s="103" t="s">
         <v>86</v>
       </c>
-      <c r="F17" s="85" t="s">
+      <c r="F17" s="104" t="s">
         <v>101</v>
       </c>
-      <c r="G17" s="80"/>
+      <c r="G17" s="105"/>
     </row>
     <row r="18" spans="1:7" ht="107.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="55" t="s">
+      <c r="A18" s="100" t="s">
         <v>87</v>
       </c>
-      <c r="B18" s="58"/>
-      <c r="C18" s="56" t="s">
+      <c r="B18" s="106"/>
+      <c r="C18" s="102" t="s">
         <v>88</v>
       </c>
-      <c r="D18" s="53" t="s">
+      <c r="D18" s="103" t="s">
         <v>89</v>
       </c>
-      <c r="E18" s="53" t="s">
+      <c r="E18" s="103" t="s">
         <v>90</v>
       </c>
-      <c r="F18" s="85" t="s">
+      <c r="F18" s="104" t="s">
         <v>103</v>
       </c>
-      <c r="G18" s="84"/>
+      <c r="G18" s="107"/>
     </row>
     <row r="19" spans="1:7" ht="177" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A19" s="54" t="s">
-        <v>108</v>
-      </c>
-      <c r="B19" s="86">
+      <c r="A19" s="109" t="s">
+        <v>107</v>
+      </c>
+      <c r="B19" s="110">
         <v>7</v>
       </c>
-      <c r="C19" s="53" t="s">
+      <c r="C19" s="111" t="s">
         <v>79</v>
       </c>
-      <c r="D19" s="53" t="s">
+      <c r="D19" s="111" t="s">
         <v>77</v>
       </c>
-      <c r="E19" s="53" t="s">
+      <c r="E19" s="111" t="s">
         <v>78</v>
       </c>
-      <c r="F19" s="53" t="s">
+      <c r="F19" s="111" t="s">
         <v>98</v>
       </c>
-      <c r="G19" s="84" t="s">
-        <v>107</v>
+      <c r="G19" s="112" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="141.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="54" t="s">
+      <c r="A20" s="113" t="s">
         <v>80</v>
       </c>
-      <c r="B20" s="59">
+      <c r="B20" s="114">
         <v>8</v>
       </c>
-      <c r="C20" s="53" t="s">
-        <v>109</v>
-      </c>
-      <c r="D20" s="53" t="s">
+      <c r="C20" s="115" t="s">
+        <v>108</v>
+      </c>
+      <c r="D20" s="115" t="s">
         <v>81</v>
       </c>
-      <c r="E20" s="53" t="s">
+      <c r="E20" s="115" t="s">
         <v>82</v>
       </c>
-      <c r="F20" s="85" t="s">
+      <c r="F20" s="116" t="s">
         <v>99</v>
       </c>
-      <c r="G20" s="80" t="s">
-        <v>107</v>
+      <c r="G20" s="81" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="149.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="55"/>
-      <c r="B21" s="58"/>
-      <c r="C21" s="56" t="s">
+      <c r="A21" s="117"/>
+      <c r="B21" s="118"/>
+      <c r="C21" s="119" t="s">
         <v>95</v>
       </c>
-      <c r="D21" s="53" t="s">
+      <c r="D21" s="115" t="s">
         <v>97</v>
       </c>
-      <c r="E21" s="53" t="s">
+      <c r="E21" s="115" t="s">
         <v>96</v>
       </c>
-      <c r="F21" s="85" t="s">
+      <c r="F21" s="116" t="s">
         <v>102</v>
       </c>
-      <c r="G21" s="84"/>
+      <c r="G21" s="120"/>
     </row>
     <row r="22" spans="1:7" ht="105" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>

</xml_diff>